<commit_message>
Changed uncert in log to 1-uncert, added rnn log
</commit_message>
<xml_diff>
--- a/Architecture and parameter search/results/separate/epimap/summaryEpimap.xlsx
+++ b/Architecture and parameter search/results/separate/epimap/summaryEpimap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\research\deepBrain\Architecture and parameter search\results\separate\epimap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8C0BBA-7966-489A-976D-D177F5EB3C8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441677F2-F955-4A95-8C14-FC976998A9D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="673" firstSheet="11" activeTab="16" xr2:uid="{449156B2-5CB7-49EB-99A2-741F8BA8F02E}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <sheet name="summaryCr" sheetId="13" r:id="rId16"/>
     <sheet name="summaryComp" sheetId="16" r:id="rId17"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId18"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +39,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -14938,6 +14937,24 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryComp!$B$1:$E$1,summaryComp!$G$1)</c:f>
@@ -15015,6 +15032,24 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryComp!$B$1:$E$1,summaryComp!$G$1)</c:f>
@@ -15092,6 +15127,24 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryComp!$B$1:$E$1,summaryComp!$G$1)</c:f>
@@ -15453,6 +15506,24 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$4:$A$6</c:f>
@@ -15518,6 +15589,24 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$4:$A$6</c:f>
@@ -15583,6 +15672,24 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$4:$A$6</c:f>
@@ -15648,6 +15755,24 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$4:$A$6</c:f>
@@ -15713,6 +15838,24 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$4:$A$6</c:f>
@@ -38343,240 +38486,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="epimapDeepSeaChrome19"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>trainLoss</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>trainTpr</v>
-          </cell>
-          <cell r="H1" t="str">
-            <v>testLoss</v>
-          </cell>
-          <cell r="J1" t="str">
-            <v>testUncer</v>
-          </cell>
-          <cell r="K1" t="str">
-            <v>testTpr</v>
-          </cell>
-          <cell r="M1" t="str">
-            <v>testRoc</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2">
-            <v>0.42699999999999999</v>
-          </cell>
-          <cell r="E2">
-            <v>0.26500000000000001</v>
-          </cell>
-          <cell r="H2">
-            <v>0.49299999999999999</v>
-          </cell>
-          <cell r="J2">
-            <v>0.253</v>
-          </cell>
-          <cell r="K2">
-            <v>0.65300000000000002</v>
-          </cell>
-          <cell r="M2">
-            <v>0.755</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>0.40899999999999997</v>
-          </cell>
-          <cell r="E3">
-            <v>0.32600000000000001</v>
-          </cell>
-          <cell r="H3">
-            <v>0.496</v>
-          </cell>
-          <cell r="J3">
-            <v>0.22700000000000001</v>
-          </cell>
-          <cell r="K3">
-            <v>0.56299999999999994</v>
-          </cell>
-          <cell r="M3">
-            <v>0.77100000000000002</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>0.40799999999999997</v>
-          </cell>
-          <cell r="E4">
-            <v>0.32700000000000001</v>
-          </cell>
-          <cell r="H4">
-            <v>0.49399999999999999</v>
-          </cell>
-          <cell r="J4">
-            <v>0.248</v>
-          </cell>
-          <cell r="K4">
-            <v>0.54200000000000004</v>
-          </cell>
-          <cell r="M4">
-            <v>0.78500000000000003</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>0.40300000000000002</v>
-          </cell>
-          <cell r="E5">
-            <v>0.33500000000000002</v>
-          </cell>
-          <cell r="H5">
-            <v>0.49099999999999999</v>
-          </cell>
-          <cell r="J5">
-            <v>0.245</v>
-          </cell>
-          <cell r="K5">
-            <v>0.54900000000000004</v>
-          </cell>
-          <cell r="M5">
-            <v>0.79400000000000004</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>0.40100000000000002</v>
-          </cell>
-          <cell r="E6">
-            <v>0.34599999999999997</v>
-          </cell>
-          <cell r="H6">
-            <v>0.49199999999999999</v>
-          </cell>
-          <cell r="J6">
-            <v>0.23400000000000001</v>
-          </cell>
-          <cell r="K6">
-            <v>0.56799999999999995</v>
-          </cell>
-          <cell r="M6">
-            <v>0.80400000000000005</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>0.40100000000000002</v>
-          </cell>
-          <cell r="E7">
-            <v>0.34899999999999998</v>
-          </cell>
-          <cell r="H7">
-            <v>0.48899999999999999</v>
-          </cell>
-          <cell r="J7">
-            <v>0.246</v>
-          </cell>
-          <cell r="K7">
-            <v>0.56999999999999995</v>
-          </cell>
-          <cell r="M7">
-            <v>0.80300000000000005</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>0.40400000000000003</v>
-          </cell>
-          <cell r="E8">
-            <v>0.34599999999999997</v>
-          </cell>
-          <cell r="H8">
-            <v>0.48599999999999999</v>
-          </cell>
-          <cell r="J8">
-            <v>0.23200000000000001</v>
-          </cell>
-          <cell r="K8">
-            <v>0.58399999999999996</v>
-          </cell>
-          <cell r="M8">
-            <v>0.80100000000000005</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>0.40100000000000002</v>
-          </cell>
-          <cell r="E9">
-            <v>0.35199999999999998</v>
-          </cell>
-          <cell r="H9">
-            <v>0.49</v>
-          </cell>
-          <cell r="J9">
-            <v>0.23699999999999999</v>
-          </cell>
-          <cell r="K9">
-            <v>0.56699999999999995</v>
-          </cell>
-          <cell r="M9">
-            <v>0.80100000000000005</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>0.4</v>
-          </cell>
-          <cell r="E10">
-            <v>0.35699999999999998</v>
-          </cell>
-          <cell r="H10">
-            <v>0.48899999999999999</v>
-          </cell>
-          <cell r="J10">
-            <v>0.22900000000000001</v>
-          </cell>
-          <cell r="K10">
-            <v>0.57799999999999996</v>
-          </cell>
-          <cell r="M10">
-            <v>0.79900000000000004</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>0.39900000000000002</v>
-          </cell>
-          <cell r="E11">
-            <v>0.36099999999999999</v>
-          </cell>
-          <cell r="H11">
-            <v>0.48799999999999999</v>
-          </cell>
-          <cell r="J11">
-            <v>0.23100000000000001</v>
-          </cell>
-          <cell r="K11">
-            <v>0.57999999999999996</v>
-          </cell>
-          <cell r="M11">
-            <v>0.8</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -41700,7 +41609,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Significance tests to the summaries
</commit_message>
<xml_diff>
--- a/Architecture and parameter search/results/separate/epimap/summaryEpimap.xlsx
+++ b/Architecture and parameter search/results/separate/epimap/summaryEpimap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\research\deepBrain\Architecture and parameter search\results\separate\epimap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AC622B-BFCF-4134-8B40-A4DD0F93E26C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60721741-B5FF-4312-A525-79E8BEEC3D31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="673" firstSheet="11" activeTab="18" xr2:uid="{449156B2-5CB7-49EB-99A2-741F8BA8F02E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="673" firstSheet="12" activeTab="20" xr2:uid="{449156B2-5CB7-49EB-99A2-741F8BA8F02E}"/>
   </bookViews>
   <sheets>
     <sheet name="Exp Description" sheetId="9" r:id="rId1"/>
@@ -32,10 +32,9 @@
     <sheet name="epimapRnn_cr19" sheetId="21" r:id="rId17"/>
     <sheet name="summaryOpt" sheetId="8" r:id="rId18"/>
     <sheet name="summaryComp" sheetId="16" r:id="rId19"/>
+    <sheet name="ttest" sheetId="22" r:id="rId20"/>
+    <sheet name="anova" sheetId="23" r:id="rId21"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId20"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="92">
   <si>
     <t>trainLoss</t>
   </si>
@@ -205,12 +204,138 @@
   <si>
     <t xml:space="preserve">  </t>
   </si>
+  <si>
+    <t>Variable 1</t>
+  </si>
+  <si>
+    <t>Variable 2</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Pearson Correlation</t>
+  </si>
+  <si>
+    <t>Hypothesized Mean Difference</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) one-tail</t>
+  </si>
+  <si>
+    <t>t Critical one-tail</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) two-tail</t>
+  </si>
+  <si>
+    <t>t Critical two-tail</t>
+  </si>
+  <si>
+    <t>exp8 vs deepsea t-Test: Paired Two Sample for Means</t>
+  </si>
+  <si>
+    <t>alpha = 0.05</t>
+  </si>
+  <si>
+    <t>difference not significant since: P two tail &gt;= alpha (0.05)</t>
+  </si>
+  <si>
+    <t>exp8 vs rnn t-Test: Paired Two Sample for Means</t>
+  </si>
+  <si>
+    <t>difference is significant since: P two tail &lt; alpha (0.05)</t>
+  </si>
+  <si>
+    <t>deepsea vs rnn t-Test: Paired Two Sample for Means</t>
+  </si>
+  <si>
+    <t>alpha = 0.01</t>
+  </si>
+  <si>
+    <t>difference not significant since: P two tail &gt;= alpha (0.01)</t>
+  </si>
+  <si>
+    <t>difference is significant since: P two tail &lt; alpha (0.01)</t>
+  </si>
+  <si>
+    <t>Anova: Single Factor</t>
+  </si>
+  <si>
+    <t>SUMMARY</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Column 1</t>
+  </si>
+  <si>
+    <t>Column 2</t>
+  </si>
+  <si>
+    <t>Column 3</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Source of Variation</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>F crit</t>
+  </si>
+  <si>
+    <t>Between Groups</t>
+  </si>
+  <si>
+    <t>Within Groups</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>F &gt; F crit =&gt; reject null hypothesis, at least one mean TPR is different</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,16 +352,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -244,13 +391,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -47006,16 +47185,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>471487</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -47043,15 +47222,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -47081,15 +47260,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>466724</xdr:colOff>
+      <xdr:colOff>600074</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -47116,16 +47295,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -47877,240 +48056,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="epimapRnn_cr19"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>trainLoss</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>trainTpr</v>
-          </cell>
-          <cell r="H1" t="str">
-            <v>testLoss</v>
-          </cell>
-          <cell r="J1" t="str">
-            <v>1-testUncer</v>
-          </cell>
-          <cell r="K1" t="str">
-            <v>testTpr</v>
-          </cell>
-          <cell r="M1" t="str">
-            <v>testRoc</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2">
-            <v>0.504</v>
-          </cell>
-          <cell r="E2">
-            <v>8.2000000000000003E-2</v>
-          </cell>
-          <cell r="H2">
-            <v>0.52600000000000002</v>
-          </cell>
-          <cell r="J2">
-            <v>0.79300000000000004</v>
-          </cell>
-          <cell r="K2">
-            <v>7.0000000000000007E-2</v>
-          </cell>
-          <cell r="M2">
-            <v>0.49399999999999999</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>0.49</v>
-          </cell>
-          <cell r="E3">
-            <v>7.9000000000000001E-2</v>
-          </cell>
-          <cell r="H3">
-            <v>0.52400000000000002</v>
-          </cell>
-          <cell r="J3">
-            <v>0.79300000000000004</v>
-          </cell>
-          <cell r="K3">
-            <v>8.1000000000000003E-2</v>
-          </cell>
-          <cell r="M3">
-            <v>0.49399999999999999</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>0.48899999999999999</v>
-          </cell>
-          <cell r="E4">
-            <v>0.08</v>
-          </cell>
-          <cell r="H4">
-            <v>0.52400000000000002</v>
-          </cell>
-          <cell r="J4">
-            <v>0.78700000000000003</v>
-          </cell>
-          <cell r="K4">
-            <v>7.0000000000000007E-2</v>
-          </cell>
-          <cell r="M4">
-            <v>0.495</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>0.48799999999999999</v>
-          </cell>
-          <cell r="E5">
-            <v>0.08</v>
-          </cell>
-          <cell r="H5">
-            <v>0.52400000000000002</v>
-          </cell>
-          <cell r="J5">
-            <v>0.79300000000000004</v>
-          </cell>
-          <cell r="K5">
-            <v>8.1000000000000003E-2</v>
-          </cell>
-          <cell r="M5">
-            <v>0.495</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>0.48799999999999999</v>
-          </cell>
-          <cell r="E6">
-            <v>0.08</v>
-          </cell>
-          <cell r="H6">
-            <v>0.52400000000000002</v>
-          </cell>
-          <cell r="J6">
-            <v>0.79300000000000004</v>
-          </cell>
-          <cell r="K6">
-            <v>8.1000000000000003E-2</v>
-          </cell>
-          <cell r="M6">
-            <v>0.49199999999999999</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>0.48799999999999999</v>
-          </cell>
-          <cell r="E7">
-            <v>7.9000000000000001E-2</v>
-          </cell>
-          <cell r="H7">
-            <v>0.52400000000000002</v>
-          </cell>
-          <cell r="J7">
-            <v>0.79300000000000004</v>
-          </cell>
-          <cell r="K7">
-            <v>8.1000000000000003E-2</v>
-          </cell>
-          <cell r="M7">
-            <v>0.49399999999999999</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>0.48899999999999999</v>
-          </cell>
-          <cell r="E8">
-            <v>0.08</v>
-          </cell>
-          <cell r="H8">
-            <v>0.52400000000000002</v>
-          </cell>
-          <cell r="J8">
-            <v>0.79300000000000004</v>
-          </cell>
-          <cell r="K8">
-            <v>8.1000000000000003E-2</v>
-          </cell>
-          <cell r="M8">
-            <v>0.49399999999999999</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>0.48799999999999999</v>
-          </cell>
-          <cell r="E9">
-            <v>7.9000000000000001E-2</v>
-          </cell>
-          <cell r="H9">
-            <v>0.52400000000000002</v>
-          </cell>
-          <cell r="J9">
-            <v>0.79300000000000004</v>
-          </cell>
-          <cell r="K9">
-            <v>7.0000000000000007E-2</v>
-          </cell>
-          <cell r="M9">
-            <v>0.49399999999999999</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>0.49</v>
-          </cell>
-          <cell r="E10">
-            <v>7.9000000000000001E-2</v>
-          </cell>
-          <cell r="H10">
-            <v>0.52400000000000002</v>
-          </cell>
-          <cell r="J10">
-            <v>0.79300000000000004</v>
-          </cell>
-          <cell r="K10">
-            <v>7.0000000000000007E-2</v>
-          </cell>
-          <cell r="M10">
-            <v>0.495</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>0.48499999999999999</v>
-          </cell>
-          <cell r="E11">
-            <v>0.08</v>
-          </cell>
-          <cell r="H11">
-            <v>0.52400000000000002</v>
-          </cell>
-          <cell r="J11">
-            <v>0.79300000000000004</v>
-          </cell>
-          <cell r="K11">
-            <v>7.0000000000000007E-2</v>
-          </cell>
-          <cell r="M11">
-            <v>0.49299999999999999</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -52555,10 +52500,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1356B018-0FE6-4F42-9650-4057796C55F9}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:V26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52566,7 +52511,7 @@
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -52586,12 +52531,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -52614,7 +52559,7 @@
         <v>0.77300000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -52637,7 +52582,7 @@
         <v>0.75900000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -52660,12 +52605,36 @@
         <v>0.80600000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -52688,7 +52657,7 @@
         <v>0.74350000000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -52711,7 +52680,7 @@
         <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -52734,12 +52703,36 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -52762,7 +52755,7 @@
         <v>0.4945</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -52785,7 +52778,7 @@
         <v>0.49099999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -53279,6 +53272,956 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF462BF1-3F0B-4CB2-B93A-7991B7A7083F}">
+  <dimension ref="A1:Z50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="6" max="6" width="50.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.62233333333333329</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.43216666666666664</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.62233333333333329</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.43216666666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="2">
+        <v>8.9763333333333639E-3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.6391083333333334E-2</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="2">
+        <v>8.9763333333333639E-3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.6391083333333334E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.77267751197540513</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.77267751197540513</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4.0474482578293944</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="2">
+        <v>4.0474482578293944</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2.7983859235353514E-2</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2.7983859235353514E-2</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.9199855803537269</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="2">
+        <v>6.9645567342832733</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="2">
+        <v>5.5967718470707029E-2</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5.5967718470707029E-2</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4.3026527297494637</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="3">
+        <v>9.9248432009182928</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.62233333333333329</v>
+      </c>
+      <c r="C21" s="2">
+        <v>7.4666666666666673E-2</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.62233333333333329</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7.4666666666666673E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="2">
+        <v>8.9763333333333639E-3</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.6033333333333351E-4</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="2">
+        <v>8.9763333333333639E-3</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1.6033333333333351E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="2">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="2">
+        <v>3</v>
+      </c>
+      <c r="H23" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.3531529994428132</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.3531529994428132</v>
+      </c>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="F25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="2">
+        <v>2</v>
+      </c>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="2">
+        <v>10.41878639094112</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="2">
+        <v>10.41878639094112</v>
+      </c>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="2">
+        <v>4.5434377641252527E-3</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="2">
+        <v>4.5434377641252527E-3</v>
+      </c>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2.9199855803537269</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="2">
+        <v>6.9645567342832733</v>
+      </c>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="2">
+        <v>9.0868755282505053E-3</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="F30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="2">
+        <v>9.0868755282505053E-3</v>
+      </c>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="3">
+        <v>4.3026527297494637</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" s="3">
+        <v>9.9248432009182928</v>
+      </c>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="9"/>
+    </row>
+    <row r="35" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X36" s="8"/>
+      <c r="Y36" s="8"/>
+      <c r="Z36" s="8"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.43216666666666664</v>
+      </c>
+      <c r="C38" s="2">
+        <v>7.4666666666666673E-2</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.43216666666666664</v>
+      </c>
+      <c r="H38" s="2">
+        <v>7.4666666666666673E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1.6391083333333334E-2</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1.6033333333333351E-4</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G39" s="2">
+        <v>1.6391083333333334E-2</v>
+      </c>
+      <c r="H39" s="2">
+        <v>1.6033333333333351E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="2">
+        <v>3</v>
+      </c>
+      <c r="C40" s="2">
+        <v>3</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G40" s="2">
+        <v>3</v>
+      </c>
+      <c r="H40" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="2">
+        <v>-0.32102248828903857</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="F41" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G41" s="2">
+        <v>-0.32102248828903857</v>
+      </c>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="F42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="2">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G43" s="2">
+        <v>2</v>
+      </c>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="2">
+        <v>4.6684851259817686</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="F44" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G44" s="2">
+        <v>4.6684851259817686</v>
+      </c>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2.147417584113347E-2</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="F45" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G45" s="2">
+        <v>2.147417584113347E-2</v>
+      </c>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="2">
+        <v>2.9199855803537269</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="F46" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G46" s="2">
+        <v>6.9645567342832733</v>
+      </c>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="2">
+        <v>4.294835168226694E-2</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="F47" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" s="2">
+        <v>4.294835168226694E-2</v>
+      </c>
+      <c r="H47" s="2"/>
+      <c r="X47" s="7"/>
+      <c r="Y47" s="7"/>
+      <c r="Z47" s="7"/>
+    </row>
+    <row r="48" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="3">
+        <v>4.3026527297494637</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="F48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G48" s="3">
+        <v>9.9248432009182928</v>
+      </c>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>67</v>
+      </c>
+      <c r="F50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376569C3-524D-4834-9E58-FB99610266D1}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="61.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.867</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.62233333333333329</v>
+      </c>
+      <c r="E5" s="2">
+        <v>8.9763333333333639E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.2965</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.43216666666666664</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.6391083333333334E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.224</v>
+      </c>
+      <c r="D7" s="3">
+        <v>7.4666666666666673E-2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.6033333333333351E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.46390838888888891</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.23195419444444446</v>
+      </c>
+      <c r="E12" s="2">
+        <v>27.259064482115875</v>
+      </c>
+      <c r="F12" s="2">
+        <v>9.7453462396347398E-4</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5.1432528497847176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="2">
+        <v>5.1055499999999983E-2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2">
+        <v>8.5092499999999977E-3</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.51496388888888889</v>
+      </c>
+      <c r="C15" s="3">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB849E1-4FF7-4E7C-9E6E-F97EE8DD0ECC}">
   <dimension ref="A1:M11"/>

</xml_diff>

<commit_message>
Added final report to present to group
</commit_message>
<xml_diff>
--- a/Architecture and parameter search/results/separate/epimap/summaryEpimap.xlsx
+++ b/Architecture and parameter search/results/separate/epimap/summaryEpimap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\research\deepBrain\Architecture and parameter search\results\separate\epimap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60721741-B5FF-4312-A525-79E8BEEC3D31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265C42B3-6A9D-472C-BC63-0B512D1FA907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="673" firstSheet="12" activeTab="20" xr2:uid="{449156B2-5CB7-49EB-99A2-741F8BA8F02E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="673" firstSheet="12" activeTab="18" xr2:uid="{449156B2-5CB7-49EB-99A2-741F8BA8F02E}"/>
   </bookViews>
   <sheets>
     <sheet name="Exp Description" sheetId="9" r:id="rId1"/>
@@ -52502,7 +52502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1356B018-0FE6-4F42-9650-4057796C55F9}">
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:V26"/>
     </sheetView>
   </sheetViews>
@@ -54029,7 +54029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376569C3-524D-4834-9E58-FB99610266D1}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated presentation file and its supps
</commit_message>
<xml_diff>
--- a/Architecture and parameter search/results/separate/epimap/summaryEpimap.xlsx
+++ b/Architecture and parameter search/results/separate/epimap/summaryEpimap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\research\deepBrain\Architecture and parameter search\results\separate\epimap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Research\deepbrain\git\deepBrain\Architecture and parameter search\results\separate\epimap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265C42B3-6A9D-472C-BC63-0B512D1FA907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C593DF26-9837-46ED-A2C9-2752940ACA7F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="673" firstSheet="12" activeTab="18" xr2:uid="{449156B2-5CB7-49EB-99A2-741F8BA8F02E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="673" firstSheet="13" activeTab="17" xr2:uid="{449156B2-5CB7-49EB-99A2-741F8BA8F02E}"/>
   </bookViews>
   <sheets>
     <sheet name="Exp Description" sheetId="9" r:id="rId1"/>
@@ -15249,24 +15249,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryOpt!$A$2:$A$10</c:f>
@@ -15368,24 +15350,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryOpt!$A$2:$A$10</c:f>
@@ -15487,24 +15451,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryOpt!$A$2:$A$10</c:f>
@@ -15606,24 +15552,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryOpt!$A$2:$A$10</c:f>
@@ -15725,24 +15653,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryOpt!$A$2:$A$10</c:f>
@@ -16128,24 +16038,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryOpt!$B$1:$E$1,summaryOpt!$G$1)</c:f>
@@ -16223,24 +16115,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryOpt!$B$1:$E$1,summaryOpt!$G$1)</c:f>
@@ -16318,24 +16192,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryOpt!$B$1:$E$1,summaryOpt!$G$1)</c:f>
@@ -16413,24 +16269,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryOpt!$B$1:$E$1,summaryOpt!$G$1)</c:f>
@@ -16508,24 +16346,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryOpt!$B$1:$E$1,summaryOpt!$G$1)</c:f>
@@ -16603,24 +16423,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryOpt!$B$1:$E$1,summaryOpt!$G$1)</c:f>
@@ -16700,24 +16502,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryOpt!$B$1:$E$1,summaryOpt!$G$1)</c:f>
@@ -16797,24 +16581,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryOpt!$B$1:$E$1,summaryOpt!$G$1)</c:f>
@@ -16894,24 +16660,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryOpt!$B$1:$E$1,summaryOpt!$G$1)</c:f>
@@ -17273,24 +17021,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryComp!$B$1:$E$1,summaryComp!$G$1)</c:f>
@@ -17368,24 +17098,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryComp!$B$1:$E$1,summaryComp!$G$1)</c:f>
@@ -17463,24 +17175,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryComp!$B$1:$E$1,summaryComp!$G$1)</c:f>
@@ -17842,24 +17536,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$15:$A$17</c:f>
@@ -17925,24 +17601,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$15:$A$17</c:f>
@@ -18008,24 +17666,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$15:$A$17</c:f>
@@ -18091,24 +17731,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$15:$A$17</c:f>
@@ -18174,24 +17796,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$15:$A$17</c:f>
@@ -18541,24 +18145,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryComp!$B$1:$E$1,summaryComp!$G$1)</c:f>
@@ -18636,24 +18222,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryComp!$B$1:$E$1,summaryComp!$G$1)</c:f>
@@ -18731,24 +18299,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryComp!$B$1:$E$1,summaryComp!$G$1)</c:f>
@@ -19110,24 +18660,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$4:$A$6</c:f>
@@ -19193,24 +18725,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$4:$A$6</c:f>
@@ -19276,24 +18790,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$4:$A$6</c:f>
@@ -19359,24 +18855,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$4:$A$6</c:f>
@@ -19442,24 +18920,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$4:$A$6</c:f>
@@ -19809,24 +19269,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryComp!$B$1:$E$1,summaryComp!$G$1)</c:f>
@@ -19904,24 +19346,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryComp!$B$1:$E$1,summaryComp!$G$1)</c:f>
@@ -19999,24 +19423,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(summaryComp!$B$1:$E$1,summaryComp!$G$1)</c:f>
@@ -20942,24 +20348,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$28:$A$30</c:f>
@@ -21025,24 +20413,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$28:$A$30</c:f>
@@ -21108,24 +20478,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>summaryComp!$A$28:$A$30</c:f>
@@ -52259,8 +51611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026925B1-A343-4BF5-BE06-4C4D36A4A9CD}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52502,8 +51854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1356B018-0FE6-4F42-9650-4057796C55F9}">
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:V26"/>
+    <sheetView topLeftCell="G20" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>